<commit_message>
Adding cost estimate to sheet
</commit_message>
<xml_diff>
--- a/PR_components/OverallBalance.xlsx
+++ b/PR_components/OverallBalance.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wylie/Desktop/UW/CHEME485_ProcessDesign/Wi2020_CHEME485_FinalProject/PR_components/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kauib\ChemE485\Wi2020_CHEME485_FinalProject\PR_components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BDDE210-3176-984F-9AF3-7FC0EB7E0873}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C893C82E-7DA8-4F9E-A688-D002A1F446F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{D3024984-B56B-EB48-83B5-18E37269D281}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D3024984-B56B-EB48-83B5-18E37269D281}"/>
   </bookViews>
   <sheets>
     <sheet name="Mass Balance" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="77">
   <si>
     <t>Assumptions</t>
   </si>
@@ -234,16 +234,47 @@
   </si>
   <si>
     <t>No recycle</t>
+  </si>
+  <si>
+    <t>12 - kg</t>
+  </si>
+  <si>
+    <t>Preliminary Cost Analysis</t>
+  </si>
+  <si>
+    <t>MW (g/mol)</t>
+  </si>
+  <si>
+    <t>Molar Flow (mol</t>
+  </si>
+  <si>
+    <t>Flowrate (ton/year)</t>
+  </si>
+  <si>
+    <t>Price ($/ton)</t>
+  </si>
+  <si>
+    <t>Cost (mil $)</t>
+  </si>
+  <si>
+    <t>Intratec, May 2007</t>
+  </si>
+  <si>
+    <t>Annual In-Out Estimate</t>
+  </si>
+  <si>
+    <t>million $</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -290,15 +321,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -306,23 +343,67 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="9">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -409,7 +490,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A2B202C9-A0AF-574C-A1A6-EA5F187381FF}" name="Table1" displayName="Table1" ref="A9:E22" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A2B202C9-A0AF-574C-A1A6-EA5F187381FF}" name="Table1" displayName="Table1" ref="A9:E22" totalsRowShown="0" headerRowDxfId="8">
   <autoFilter ref="A9:E22" xr:uid="{A7DD0F94-9125-8B43-B142-A6E307B43FE7}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{C95DAD9F-9D62-DA42-96A5-FDAFC7DDADBF}" name="Type"/>
@@ -423,10 +504,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2537B7B7-52D7-2146-BF3C-37BCFCE55006}" name="Table2" displayName="Table2" ref="A25:N32" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A25:N32" xr:uid="{0F758C04-AAF9-CA4C-93B8-83054D68DD35}"/>
-  <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{78705F38-D8A6-6C4A-B060-7D18603E2F3F}" name="Components" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2537B7B7-52D7-2146-BF3C-37BCFCE55006}" name="Table2" displayName="Table2" ref="A25:O32" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="A25:O32" xr:uid="{0F758C04-AAF9-CA4C-93B8-83054D68DD35}"/>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{78705F38-D8A6-6C4A-B060-7D18603E2F3F}" name="Components" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{B92D258C-C62E-ED49-A04B-4B05DB6A0544}" name="1"/>
     <tableColumn id="3" xr3:uid="{EF715E3C-D341-D44C-BEF7-20F1EB1F51C7}" name="2"/>
     <tableColumn id="4" xr3:uid="{2984E2FB-CBB0-2F49-9466-E71E03D1615C}" name="3">
@@ -446,19 +527,43 @@
     <tableColumn id="14" xr3:uid="{F5FD682B-397F-4A45-9B3B-CE2CCF13203A}" name="10 - g"/>
     <tableColumn id="12" xr3:uid="{F6746A49-92E8-6348-98CE-B63E3F4D369D}" name="11 - g"/>
     <tableColumn id="13" xr3:uid="{795745FF-80D3-3C4E-BEA3-8C1D4AEBBBF5}" name="12 - g"/>
+    <tableColumn id="15" xr3:uid="{4BA2BA1F-EAD3-468B-92E5-42EE7BFEADD0}" name="12 - kg" dataDxfId="4">
+      <calculatedColumnFormula>Table2[[#This Row],[12 - g]]/1000000</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{718CE5DA-D8E2-844A-A7B3-3FDA691942DD}" name="Table3" displayName="Table3" ref="G9:J13" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{718CE5DA-D8E2-844A-A7B3-3FDA691942DD}" name="Table3" displayName="Table3" ref="G9:J13" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="G9:J13" xr:uid="{69EA015C-F368-AC4C-BF5B-49D7A5D8C214}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{27866C21-9878-1840-86B0-F473DB7F465B}" name="Species"/>
     <tableColumn id="2" xr3:uid="{6AE8B7EC-6122-294B-9E8E-116A991F4443}" name="Property"/>
     <tableColumn id="3" xr3:uid="{112ACDC3-4916-D149-A524-3C87984CC1B9}" name="Value"/>
     <tableColumn id="4" xr3:uid="{5554A68B-003A-2F45-A098-6F62897DB683}" name="Units"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E599246E-8815-4DF0-BC90-6C76702B4DF4}" name="Table14" displayName="Table14" ref="A35:F38" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A35:F38" xr:uid="{F4FFC18F-BA09-444F-8336-1FCBE5EECCE9}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{0677A384-1FCC-4BBA-B820-5958FB10E855}" name="Components"/>
+    <tableColumn id="2" xr3:uid="{0C9DFF9B-7E20-471C-A636-9342216E87F6}" name="MW (g/mol)"/>
+    <tableColumn id="3" xr3:uid="{A9A021C3-1CAB-45F1-9632-AF34BDE6E422}" name="Molar Flow (mol" dataDxfId="2">
+      <calculatedColumnFormula>Table14[[#This Row],[Flowrate (ton/year)]]/Table14[[#This Row],[MW (g/mol)]]*1000000</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{2445DA69-7187-4359-BFC0-8E07D6278C5D}" name="Flowrate (ton/year)" dataDxfId="1">
+      <calculatedColumnFormula>N29/1000000</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{9581D998-A209-43B8-9844-3F6EE50A0E0E}" name="Price ($/ton)"/>
+    <tableColumn id="6" xr3:uid="{AC6B61D1-FE74-4601-A6AF-452236A43C28}" name="Cost (mil $)" dataDxfId="0">
+      <calculatedColumnFormula>Table14[[#This Row],[Price ($/ton)]]*Table14[[#This Row],[Flowrate (ton/year)]]/1000000</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -761,49 +866,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45065C35-D5EC-AA4A-B23B-2850BA63C6DA}">
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="55" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.6640625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" customWidth="1"/>
     <col min="5" max="5" width="21.1640625" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="13.5" customWidth="1"/>
-    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>1</v>
       </c>
@@ -811,7 +917,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
@@ -840,7 +946,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -870,7 +976,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>9</v>
       </c>
@@ -893,7 +999,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C12">
         <f>C11*I11/1000</f>
         <v>122869093.66686371</v>
@@ -914,7 +1020,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>59</v>
       </c>
@@ -937,7 +1043,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>60</v>
       </c>
@@ -948,7 +1054,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>61</v>
       </c>
@@ -959,7 +1065,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>62</v>
       </c>
@@ -970,7 +1076,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>63</v>
       </c>
@@ -981,7 +1087,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
@@ -999,7 +1105,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>11</v>
       </c>
@@ -1015,7 +1121,7 @@
       </c>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:14" s="1" customFormat="1">
+    <row r="20" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>32</v>
       </c>
@@ -1030,7 +1136,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>33</v>
       </c>
@@ -1044,7 +1150,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>34</v>
       </c>
@@ -1058,13 +1164,13 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B24" s="1"/>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>14</v>
       </c>
@@ -1107,8 +1213,11 @@
       <c r="N25" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="26" spans="1:14">
+      <c r="O25" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>15</v>
       </c>
@@ -1157,8 +1266,12 @@
       <c r="N26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:14">
+      <c r="O26">
+        <f>Table2[[#This Row],[12 - g]]/1000000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>16</v>
       </c>
@@ -1207,8 +1320,12 @@
       <c r="N27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:14">
+      <c r="O27">
+        <f>Table2[[#This Row],[12 - g]]/1000000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>17</v>
       </c>
@@ -1257,8 +1374,12 @@
       <c r="N28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:14">
+      <c r="O28">
+        <f>Table2[[#This Row],[12 - g]]/1000000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>18</v>
       </c>
@@ -1310,8 +1431,12 @@
       <c r="N29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:14">
+      <c r="O29">
+        <f>Table2[[#This Row],[12 - g]]/1000000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>19</v>
       </c>
@@ -1365,8 +1490,12 @@
         <f>L30-Table2[[#This Row],[11 - g]]</f>
         <v>100003572.27551651</v>
       </c>
-    </row>
-    <row r="31" spans="1:14">
+      <c r="O30">
+        <f>Table2[[#This Row],[12 - g]]/1000000</f>
+        <v>100.0035722755165</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>20</v>
       </c>
@@ -1419,8 +1548,12 @@
         <f>L31-Table2[[#This Row],[11 - g]]</f>
         <v>100000000000</v>
       </c>
-    </row>
-    <row r="32" spans="1:14">
+      <c r="O31">
+        <f>Table2[[#This Row],[12 - g]]/1000000</f>
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>21</v>
       </c>
@@ -1468,14 +1601,126 @@
       <c r="N32">
         <v>0</v>
       </c>
+      <c r="O32">
+        <f>Table2[[#This Row],[12 - g]]/1000000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36">
+        <v>106.16</v>
+      </c>
+      <c r="C36">
+        <f>D29</f>
+        <v>1156959450.7237637</v>
+      </c>
+      <c r="D36">
+        <f>Table14[[#This Row],[Molar Flow (mol]]*Table14[[#This Row],[MW (g/mol)]]/1000000</f>
+        <v>122822.81528883475</v>
+      </c>
+      <c r="E36">
+        <v>701</v>
+      </c>
+      <c r="F36" s="6">
+        <f>Table14[[#This Row],[Price ($/ton)]]*Table14[[#This Row],[Flowrate (ton/year)]]/1000000</f>
+        <v>86.098793517473155</v>
+      </c>
+      <c r="H36" s="7">
+        <f>F38+F37-Table14[[#This Row],[Cost (mil $)]]</f>
+        <v>38.944411598025397</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37">
+        <v>98.06</v>
+      </c>
+      <c r="D37">
+        <f t="shared" ref="D37" si="0">N30/1000000</f>
+        <v>100.0035722755165</v>
+      </c>
+      <c r="E37">
+        <v>1432</v>
+      </c>
+      <c r="F37" s="6">
+        <f>Table14[[#This Row],[Price ($/ton)]]*Table14[[#This Row],[Flowrate (ton/year)]]/1000000</f>
+        <v>0.14320511549853965</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38">
+        <v>148.1</v>
+      </c>
+      <c r="D38">
+        <f>N31/1000000</f>
+        <v>100000</v>
+      </c>
+      <c r="E38">
+        <v>1249</v>
+      </c>
+      <c r="F38" s="6">
+        <f>Table14[[#This Row],[Price ($/ton)]]*Table14[[#This Row],[Flowrate (ton/year)]]/1000000</f>
+        <v>124.9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E39" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A41" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="3">
+  <tableParts count="4">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updating for PFD Checkpoint
</commit_message>
<xml_diff>
--- a/PR_components/OverallBalance.xlsx
+++ b/PR_components/OverallBalance.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wylie/Desktop/UW/CHEME485_ProcessDesign/Wi2020_CHEME485_FinalProject/PR_components/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E17B105-B5E1-434E-AE31-35E4073A44EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5438C68-7C4B-B748-AFD5-1FA0810CD96E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{D3024984-B56B-EB48-83B5-18E37269D281}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{D3024984-B56B-EB48-83B5-18E37269D281}"/>
   </bookViews>
   <sheets>
     <sheet name="Mass Balance" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="84">
   <si>
     <t>Assumptions</t>
   </si>
@@ -185,9 +186,6 @@
     <t>Units</t>
   </si>
   <si>
-    <t>Between 2.46 and 4.29</t>
-  </si>
-  <si>
     <t>PA</t>
   </si>
   <si>
@@ -264,6 +262,30 @@
   </si>
   <si>
     <t>million $</t>
+  </si>
+  <si>
+    <t>n2</t>
+  </si>
+  <si>
+    <t>Co2</t>
+  </si>
+  <si>
+    <t>Ox</t>
+  </si>
+  <si>
+    <t>PA Purity</t>
+  </si>
+  <si>
+    <t>MA Purity</t>
+  </si>
+  <si>
+    <t>OXY</t>
+  </si>
+  <si>
+    <t>PA Prod</t>
+  </si>
+  <si>
+    <t>MA Prod</t>
   </si>
 </sst>
 </file>
@@ -866,10 +888,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45065C35-D5EC-AA4A-B23B-2850BA63C6DA}">
-  <dimension ref="A1:O41"/>
+  <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="M39" sqref="M39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I29" sqref="I29:I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
@@ -902,12 +924,12 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -952,17 +974,14 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C10">
         <f>15</f>
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>58</v>
-      </c>
-      <c r="E10" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="G10" t="s">
         <v>43</v>
@@ -1006,10 +1025,10 @@
         <v>122869093.66686371</v>
       </c>
       <c r="D12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H12" t="s">
         <v>44</v>
@@ -1023,7 +1042,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="B13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C13">
         <v>0.6</v>
@@ -1032,7 +1051,7 @@
         <v>35</v>
       </c>
       <c r="G13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H13" t="s">
         <v>44</v>
@@ -1046,7 +1065,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="B14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C14">
         <v>0.3</v>
@@ -1057,10 +1076,10 @@
     </row>
     <row r="15" spans="1:10">
       <c r="B15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C15">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="E15" t="s">
         <v>37</v>
@@ -1068,10 +1087,10 @@
     </row>
     <row r="16" spans="1:10">
       <c r="B16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C16">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="E16" t="s">
         <v>38</v>
@@ -1079,10 +1098,10 @@
     </row>
     <row r="17" spans="1:15">
       <c r="B17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C17">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="E17" t="s">
         <v>39</v>
@@ -1128,7 +1147,7 @@
       </c>
       <c r="C20">
         <f>C15*E29</f>
-        <v>11569594.507237637</v>
+        <v>1156959.4507237638</v>
       </c>
       <c r="D20" t="s">
         <v>12</v>
@@ -1142,7 +1161,7 @@
         <v>33</v>
       </c>
       <c r="C21">
-        <v>10000</v>
+        <v>5</v>
       </c>
       <c r="D21" t="s">
         <v>12</v>
@@ -1156,7 +1175,7 @@
         <v>34</v>
       </c>
       <c r="C22">
-        <v>10000</v>
+        <v>5</v>
       </c>
       <c r="D22" t="s">
         <v>12</v>
@@ -1203,19 +1222,19 @@
         <v>31</v>
       </c>
       <c r="K25" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L25" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="L25" s="1" t="s">
+      <c r="M25" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="M25" s="1" t="s">
+      <c r="N25" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="N25" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="O25" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:15">
@@ -1293,15 +1312,15 @@
       </c>
       <c r="F27">
         <f>Table2[[#This Row],[4]]-3*$C$18-(15/2)*$C$19-(21/2)*$C$20-(15/2)*$C$21-3*$C$22</f>
-        <v>-1162849247.9773827</v>
+        <v>-1053411632.3839869</v>
       </c>
       <c r="G27">
         <f>Table2[[#This Row],[5]]</f>
-        <v>-1162849247.9773827</v>
+        <v>-1053411632.3839869</v>
       </c>
       <c r="H27">
         <f>Table2[[#This Row],[6]]</f>
-        <v>-1162849247.9773827</v>
+        <v>-1053411632.3839869</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -1347,15 +1366,15 @@
       </c>
       <c r="F28">
         <f>Table2[[#This Row],[4]]+4*$C$19+C20+C21+C22</f>
-        <v>1573484852.9843187</v>
+        <v>1563052227.9278047</v>
       </c>
       <c r="G28">
         <f>Table2[[#This Row],[5]]</f>
-        <v>1573484852.9843187</v>
+        <v>1563052227.9278047</v>
       </c>
       <c r="H28">
         <f>Table2[[#This Row],[6]]</f>
-        <v>1573484852.9843187</v>
+        <v>1563052227.9278047</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -1402,23 +1421,23 @@
       </c>
       <c r="F29">
         <f>Table2[[#This Row],[4]]-$C$18-$C$19-$C$20</f>
-        <v>104126350.56513873</v>
+        <v>114538985.6216526</v>
       </c>
       <c r="G29">
         <f>Table2[[#This Row],[5]]</f>
-        <v>104126350.56513873</v>
+        <v>114538985.6216526</v>
       </c>
       <c r="H29">
         <f>0.01*Table2[[#This Row],[6]]</f>
-        <v>1041263.5056513873</v>
+        <v>1145389.8562165261</v>
       </c>
       <c r="I29">
         <f>Table2[[#This Row],[6]]-Table2[[#This Row],[7]]</f>
-        <v>103085087.05948734</v>
+        <v>113393595.76543608</v>
       </c>
       <c r="J29">
         <f>Table2[[#This Row],[8]]</f>
-        <v>103085087.05948734</v>
+        <v>113393595.76543608</v>
       </c>
       <c r="K29">
         <v>0</v>
@@ -1458,42 +1477,42 @@
       </c>
       <c r="F30">
         <f>$C$19-$C$22</f>
-        <v>347077835.21712911</v>
+        <v>347087830.21712911</v>
       </c>
       <c r="G30">
         <f>Table2[[#This Row],[5]]</f>
-        <v>347077835.21712911</v>
+        <v>347087830.21712911</v>
       </c>
       <c r="H30">
         <f>0.01*Table2[[#This Row],[6]]</f>
-        <v>3470778.3521712911</v>
+        <v>3470878.3021712913</v>
       </c>
       <c r="I30">
         <f>Table2[[#This Row],[6]]-Table2[[#This Row],[7]]</f>
-        <v>343607056.86495781</v>
+        <v>343616951.91495782</v>
       </c>
       <c r="J30">
         <v>0</v>
       </c>
       <c r="K30">
         <f>Table2[[#This Row],[8]]</f>
-        <v>343607056.86495781</v>
+        <v>343616951.91495782</v>
       </c>
       <c r="L30">
         <f>Table2[[#This Row],[10 - mol]]*I13</f>
-        <v>33879655806.884838</v>
+        <v>33880631458.814838</v>
       </c>
       <c r="M30">
         <f>19*M31</f>
-        <v>33779652234.609322</v>
+        <v>33780626472.332352</v>
       </c>
       <c r="N30">
         <f>L30-Table2[[#This Row],[11 - g]]</f>
-        <v>100003572.27551651</v>
+        <v>100004986.48248672</v>
       </c>
       <c r="O30">
         <f>Table2[[#This Row],[12 - g]]/1000000</f>
-        <v>100.0035722755165</v>
+        <v>100.00498648248673</v>
       </c>
     </row>
     <row r="31" spans="1:15">
@@ -1516,42 +1535,42 @@
       </c>
       <c r="F31">
         <f>$C$18-$C$22</f>
-        <v>694165670.43425822</v>
+        <v>694175665.43425822</v>
       </c>
       <c r="G31">
         <f>Table2[[#This Row],[5]]</f>
-        <v>694165670.43425822</v>
+        <v>694175665.43425822</v>
       </c>
       <c r="H31">
         <f>0.01*Table2[[#This Row],[6]]</f>
-        <v>6941656.7043425823</v>
+        <v>6941756.6543425824</v>
       </c>
       <c r="I31">
         <f>Table2[[#This Row],[6]]-Table2[[#This Row],[7]]</f>
-        <v>687224013.72991562</v>
+        <v>687233908.77991569</v>
       </c>
       <c r="J31">
         <v>0</v>
       </c>
       <c r="K31">
         <f>Table2[[#This Row],[8]]</f>
-        <v>687224013.72991562</v>
+        <v>687233908.77991569</v>
       </c>
       <c r="L31">
         <f>Table2[[#This Row],[10 - mol]]*I12</f>
-        <v>101777876433.4005</v>
+        <v>101779341890.30551</v>
       </c>
       <c r="M31">
         <f>(0.999/18.98)*L30-(0.001/18.998)*L31</f>
-        <v>1777876433.4004905</v>
+        <v>1777927709.0701237</v>
       </c>
       <c r="N31">
         <f>L31-Table2[[#This Row],[11 - g]]</f>
-        <v>100000000000</v>
+        <v>100001414181.23538</v>
       </c>
       <c r="O31">
         <f>Table2[[#This Row],[12 - g]]/1000000</f>
-        <v>100000</v>
+        <v>100001.41418123538</v>
       </c>
     </row>
     <row r="32" spans="1:15">
@@ -1574,15 +1593,15 @@
       </c>
       <c r="F32">
         <f>3*$C$18+4*$C$19+5*$C$20+2*$C$21+$C$22</f>
-        <v>3528756324.7074795</v>
+        <v>3476663164.4249101</v>
       </c>
       <c r="G32">
         <f>Table2[[#This Row],[5]]</f>
-        <v>3528756324.7074795</v>
+        <v>3476663164.4249101</v>
       </c>
       <c r="H32">
         <f>Table2[[#This Row],[6]]</f>
-        <v>3528756324.7074795</v>
+        <v>3476663164.4249101</v>
       </c>
       <c r="I32">
         <v>0</v>
@@ -1609,7 +1628,7 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1617,22 +1636,22 @@
         <v>14</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F35" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="H35" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I35" s="5" t="s">
         <v>5</v>
@@ -1662,10 +1681,10 @@
       </c>
       <c r="H36" s="7">
         <f>F38+F37-Table14[[#This Row],[Cost (mil $)]]</f>
-        <v>38.944411598025397</v>
+        <v>38.94617993553274</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -1677,14 +1696,14 @@
       </c>
       <c r="D37">
         <f t="shared" ref="D37" si="0">N30/1000000</f>
-        <v>100.0035722755165</v>
+        <v>100.00498648248673</v>
       </c>
       <c r="E37">
         <v>1432</v>
       </c>
       <c r="F37" s="6">
         <f>Table14[[#This Row],[Price ($/ton)]]*Table14[[#This Row],[Flowrate (ton/year)]]/1000000</f>
-        <v>0.14320511549853965</v>
+        <v>0.143207140642921</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -1696,23 +1715,65 @@
       </c>
       <c r="D38">
         <f>N31/1000000</f>
-        <v>100000</v>
+        <v>100001.41418123538</v>
       </c>
       <c r="E38">
         <v>1249</v>
       </c>
       <c r="F38" s="6">
         <f>Table14[[#This Row],[Price ($/ton)]]*Table14[[#This Row],[Flowrate (ton/year)]]/1000000</f>
-        <v>124.9</v>
+        <v>124.90176631236298</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="E39" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="3"/>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="H43">
+        <f>B26+B27+B28+C29</f>
+        <v>18511351211.580223</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="H44" t="s">
+        <v>76</v>
+      </c>
+      <c r="I44">
+        <f>E26/$H$43</f>
+        <v>0.73124999999999996</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="H45" t="s">
+        <v>16</v>
+      </c>
+      <c r="I45">
+        <f t="shared" ref="I45:I47" si="1">E27/$H$43</f>
+        <v>0.19687499999999997</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="H46" t="s">
+        <v>77</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="1"/>
+        <v>9.3749999999999979E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="H47" t="s">
+        <v>78</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="1"/>
+        <v>6.2499999999999986E-2</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -1724,4 +1785,72 @@
     <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09C5910B-5A8F-2948-8A99-9F5C2C012C91}">
+  <dimension ref="F13:K17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="13" spans="6:11">
+      <c r="G13" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" t="s">
+        <v>51</v>
+      </c>
+      <c r="I13" t="s">
+        <v>81</v>
+      </c>
+      <c r="J13" t="s">
+        <v>79</v>
+      </c>
+      <c r="K13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="6:11">
+      <c r="F14" t="s">
+        <v>82</v>
+      </c>
+      <c r="G14">
+        <v>12182.3</v>
+      </c>
+      <c r="H14">
+        <v>52.378999999999998</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <f>G14/SUM(G14:I14)</f>
+        <v>0.99571880880569075</v>
+      </c>
+    </row>
+    <row r="17" spans="6:11">
+      <c r="F17" t="s">
+        <v>83</v>
+      </c>
+      <c r="G17">
+        <v>147.69999999999999</v>
+      </c>
+      <c r="H17">
+        <v>2158.5</v>
+      </c>
+      <c r="I17">
+        <v>13.986000000000001</v>
+      </c>
+      <c r="K17">
+        <f>H17/SUM(G17:I17)</f>
+        <v>0.93031334556798473</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>